<commit_message>
Carga 201511 Noviembre de 2015
</commit_message>
<xml_diff>
--- a/project_files/files/templates/rep_mtro_clientes.xlsx
+++ b/project_files/files/templates/rep_mtro_clientes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
   <si>
     <t>Empresa</t>
   </si>
@@ -132,6 +132,24 @@
   </si>
   <si>
     <t>Fecha Estatus</t>
+  </si>
+  <si>
+    <t>Fecha Servicios Inicio</t>
+  </si>
+  <si>
+    <t>Tipo de Servicio</t>
+  </si>
+  <si>
+    <t>Tipo de Cobro</t>
+  </si>
+  <si>
+    <t>Precio</t>
+  </si>
+  <si>
+    <t>kilos Integrados</t>
+  </si>
+  <si>
+    <t>Kilo Excedido</t>
   </si>
 </sst>
 </file>
@@ -464,7 +482,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW1"/>
+  <dimension ref="A1:BC1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -496,31 +514,37 @@
     <col min="25" max="25" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="9" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="10" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="28" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="9" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="21" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="9" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:55" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -603,70 +627,88 @@
         <v>26</v>
       </c>
       <c r="AB1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>35</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>